<commit_message>
test commit following issues with RStudio/ Git interfacing
</commit_message>
<xml_diff>
--- a/data files/Fe-SSA_Plaas.xlsx
+++ b/data files/Fe-SSA_Plaas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\My Drive\Fe-SSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\My Drive\Code Repositories\R\FeSSA\data files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9269B7D7-9CA7-404C-AA5C-9D1E08F0B6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFAD97B-C1BD-419D-9621-4D464AE372FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="40">
   <si>
     <t>ATOFMS Time Bins</t>
   </si>
@@ -211,7 +211,7 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>AGEDFESSA</t>
+    <t>FEAGEDSSA</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -510,6 +510,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -517,25 +518,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -929,18 +911,18 @@
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="39" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="42"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -10045,32 +10027,32 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="40" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="41"/>
-      <c r="K10" s="39" t="s">
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="42"/>
+      <c r="K10" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="39" t="s">
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="40"/>
-      <c r="S10" s="40"/>
-      <c r="T10" s="41"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="42"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
@@ -10302,10 +10284,10 @@
       <c r="M14" s="25">
         <v>2.4999999999999998E-12</v>
       </c>
-      <c r="N14" s="42">
+      <c r="N14" s="25">
         <v>2.8000000000000002E-12</v>
       </c>
-      <c r="O14" s="43">
+      <c r="O14" s="27">
         <f t="shared" si="0"/>
         <v>2.848E-12</v>
       </c>
@@ -10366,10 +10348,10 @@
       <c r="M15" s="25">
         <v>2.5999999999999998E-12</v>
       </c>
-      <c r="N15" s="42">
+      <c r="N15" s="25">
         <v>3.0000000000000001E-12</v>
       </c>
-      <c r="O15" s="43">
+      <c r="O15" s="27">
         <f t="shared" si="0"/>
         <v>2.9279999999999996E-12</v>
       </c>
@@ -10430,10 +10412,10 @@
       <c r="M16" s="25">
         <v>1.4000000000000001E-12</v>
       </c>
-      <c r="N16" s="42">
+      <c r="N16" s="25">
         <v>1.5000000000000001E-12</v>
       </c>
-      <c r="O16" s="43">
+      <c r="O16" s="27">
         <f t="shared" si="0"/>
         <v>1.485E-12</v>
       </c>
@@ -12350,10 +12332,10 @@
       <c r="M46" s="25">
         <v>1.7E-14</v>
       </c>
-      <c r="N46" s="42">
+      <c r="N46" s="25">
         <v>2.8000000000000001E-14</v>
       </c>
-      <c r="O46" s="43">
+      <c r="O46" s="27">
         <f t="shared" si="0"/>
         <v>2.7799999999999999E-14</v>
       </c>
@@ -12730,18 +12712,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="41"/>
-      <c r="F1" s="39" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="42"/>
+      <c r="F1" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
@@ -14212,22 +14194,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41"/>
-      <c r="I1" s="39" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="42"/>
+      <c r="I1" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="42"/>
     </row>
     <row r="2" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
@@ -14252,10 +14234,9 @@
       <c r="F2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="44"/>
       <c r="I2" s="9" t="str">
         <f>'Daily Resolution'!P11</f>
         <v>FEANTOTSRF</v>
@@ -14275,12 +14256,12 @@
       <c r="M2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="44" t="s">
+      <c r="N2" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="46">
+      <c r="A3" s="39">
         <v>43412</v>
       </c>
       <c r="B3" s="32">
@@ -14332,7 +14313,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="46">
+      <c r="A4" s="39">
         <v>43413</v>
       </c>
       <c r="B4" s="32">
@@ -14384,7 +14365,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="46">
+      <c r="A5" s="39">
         <v>43414</v>
       </c>
       <c r="B5" s="32">
@@ -14436,7 +14417,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="46">
+      <c r="A6" s="39">
         <v>43415</v>
       </c>
       <c r="B6" s="32">
@@ -14488,7 +14469,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="46">
+      <c r="A7" s="39">
         <v>43416</v>
       </c>
       <c r="B7" s="32">
@@ -14540,7 +14521,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="46">
+      <c r="A8" s="39">
         <v>43417</v>
       </c>
       <c r="B8" s="32">
@@ -14592,7 +14573,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="46">
+      <c r="A9" s="39">
         <v>43418</v>
       </c>
       <c r="B9" s="32">
@@ -14644,7 +14625,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="46">
+      <c r="A10" s="39">
         <v>43419</v>
       </c>
       <c r="B10" s="32">
@@ -14696,7 +14677,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="46">
+      <c r="A11" s="39">
         <v>43420</v>
       </c>
       <c r="B11" s="32">
@@ -14748,7 +14729,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="46">
+      <c r="A12" s="39">
         <v>43421</v>
       </c>
       <c r="B12" s="32">
@@ -14800,7 +14781,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="46">
+      <c r="A13" s="39">
         <v>43422</v>
       </c>
       <c r="B13" s="32">
@@ -14852,7 +14833,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="46">
+      <c r="A14" s="39">
         <v>43423</v>
       </c>
       <c r="B14" s="32">
@@ -14904,7 +14885,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="46">
+      <c r="A15" s="39">
         <v>43424</v>
       </c>
       <c r="B15" s="32">
@@ -14956,7 +14937,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="46">
+      <c r="A16" s="39">
         <v>43425</v>
       </c>
       <c r="B16" s="32">
@@ -15008,7 +14989,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="46">
+      <c r="A17" s="39">
         <v>43426</v>
       </c>
       <c r="B17" s="32">
@@ -15060,7 +15041,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="46">
+      <c r="A18" s="39">
         <v>43427</v>
       </c>
       <c r="B18" s="32">
@@ -15112,7 +15093,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="46">
+      <c r="A19" s="39">
         <v>43428</v>
       </c>
       <c r="B19" s="32">
@@ -15164,7 +15145,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="46">
+      <c r="A20" s="39">
         <v>43429</v>
       </c>
       <c r="B20" s="32">
@@ -15216,7 +15197,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="46">
+      <c r="A21" s="39">
         <v>43430</v>
       </c>
       <c r="B21" s="32">
@@ -15268,7 +15249,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="46">
+      <c r="A22" s="39">
         <v>43431</v>
       </c>
       <c r="B22" s="32">
@@ -15320,7 +15301,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="46">
+      <c r="A23" s="39">
         <v>43432</v>
       </c>
       <c r="B23" s="32">
@@ -15372,7 +15353,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="46">
+      <c r="A24" s="39">
         <v>43433</v>
       </c>
       <c r="B24" s="32">
@@ -15424,7 +15405,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="46">
+      <c r="A25" s="39">
         <v>43434</v>
       </c>
       <c r="B25" s="32">
@@ -15476,7 +15457,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" s="46">
+      <c r="A26" s="39">
         <v>43435</v>
       </c>
       <c r="B26" s="32">
@@ -15528,7 +15509,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" s="46">
+      <c r="A27" s="39">
         <v>43436</v>
       </c>
       <c r="B27" s="32">
@@ -15580,7 +15561,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="46">
+      <c r="A28" s="39">
         <v>43437</v>
       </c>
       <c r="B28" s="32">
@@ -15632,7 +15613,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A29" s="46">
+      <c r="A29" s="39">
         <v>43438</v>
       </c>
       <c r="B29" s="32">
@@ -15684,7 +15665,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" s="46">
+      <c r="A30" s="39">
         <v>43439</v>
       </c>
       <c r="B30" s="32">
@@ -15736,7 +15717,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A31" s="46">
+      <c r="A31" s="39">
         <v>43440</v>
       </c>
       <c r="B31" s="32">
@@ -15788,7 +15769,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A32" s="46">
+      <c r="A32" s="39">
         <v>43441</v>
       </c>
       <c r="B32" s="32">
@@ -15840,7 +15821,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A33" s="46">
+      <c r="A33" s="39">
         <v>43442</v>
       </c>
       <c r="B33" s="32">
@@ -15892,7 +15873,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A34" s="46">
+      <c r="A34" s="39">
         <v>43443</v>
       </c>
       <c r="B34" s="32">
@@ -15944,7 +15925,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A35" s="46">
+      <c r="A35" s="39">
         <v>43444</v>
       </c>
       <c r="B35" s="32">
@@ -15996,7 +15977,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A36" s="46">
+      <c r="A36" s="39">
         <v>43445</v>
       </c>
       <c r="B36" s="32">
@@ -16048,7 +16029,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A37" s="46">
+      <c r="A37" s="39">
         <v>43446</v>
       </c>
       <c r="B37" s="32">
@@ -16100,7 +16081,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A38" s="46">
+      <c r="A38" s="39">
         <v>43447</v>
       </c>
       <c r="B38" s="32">
@@ -16152,7 +16133,7 @@
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A39" s="46">
+      <c r="A39" s="39">
         <v>43448</v>
       </c>
       <c r="B39" s="32">
@@ -16204,7 +16185,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A40" s="46">
+      <c r="A40" s="39">
         <v>43449</v>
       </c>
       <c r="B40" s="32">
@@ -16256,7 +16237,7 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A41" s="46">
+      <c r="A41" s="39">
         <v>43450</v>
       </c>
       <c r="B41" s="32">
@@ -16308,7 +16289,7 @@
       </c>
     </row>
     <row r="42" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="46">
+      <c r="A42" s="39">
         <v>43451</v>
       </c>
       <c r="B42" s="32">
@@ -16334,7 +16315,7 @@
       <c r="G42" s="37">
         <v>8.5267981502381601E-2</v>
       </c>
-      <c r="H42" s="45"/>
+      <c r="H42" s="34"/>
       <c r="I42" s="32">
         <f>(55.854*'Fe in ppbv'!F42)/(22.41)</f>
         <v>6.8511351895180335E-6</v>
@@ -16371,10 +16352,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A26F9FA6-0CF3-4B74-B2F5-4C64534B5056}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16408,927 +16389,904 @@
       <c r="F1" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="25" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="31">
-        <v>43412</v>
+        <v>43413</v>
       </c>
       <c r="B2" s="25">
-        <v>3.6194676472925462E-4</v>
+        <v>3.7487343489815651E-4</v>
       </c>
       <c r="C2" s="25">
-        <v>3.6194676472925452E-5</v>
+        <v>6.0755349793839161E-5</v>
       </c>
       <c r="D2" s="25">
-        <v>1.9390005253352926E-3</v>
+        <v>2.8438674371584283E-3</v>
       </c>
       <c r="E2" s="25">
-        <v>2.3268006304023509E-3</v>
+        <v>3.2316675422254877E-3</v>
       </c>
       <c r="F2" s="25">
-        <v>2.3371419665374725E-3</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>3</v>
+        <v>3.2794962218504241E-3</v>
+      </c>
+      <c r="G2" s="25">
+        <v>3.1858752699618301E-3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="31">
-        <v>43413</v>
+        <v>43414</v>
       </c>
       <c r="B3" s="25">
         <v>3.7487343489815651E-4</v>
       </c>
       <c r="C3" s="25">
-        <v>6.0755349793839161E-5</v>
+        <v>7.4974686979631307E-5</v>
       </c>
       <c r="D3" s="25">
-        <v>2.8438674371584283E-3</v>
+        <v>3.2316675422254877E-3</v>
       </c>
       <c r="E3" s="25">
-        <v>3.2316675422254877E-3</v>
+        <v>3.6194676472925459E-3</v>
       </c>
       <c r="F3" s="25">
-        <v>3.2794962218504241E-3</v>
+        <v>3.6815156641032756E-3</v>
       </c>
       <c r="G3" s="25">
-        <v>3.1858752699618301E-3</v>
+        <v>2.8733624669311101E-3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="31">
-        <v>43414</v>
+        <v>43415</v>
       </c>
       <c r="B4" s="25">
-        <v>3.7487343489815651E-4</v>
+        <v>3.6194676472925462E-4</v>
       </c>
       <c r="C4" s="25">
-        <v>7.4974686979631307E-5</v>
+        <v>6.2048016810729349E-5</v>
       </c>
       <c r="D4" s="25">
-        <v>3.2316675422254877E-3</v>
+        <v>3.360934243914507E-3</v>
       </c>
       <c r="E4" s="25">
-        <v>3.6194676472925459E-3</v>
+        <v>3.8780010506705852E-3</v>
       </c>
       <c r="F4" s="25">
-        <v>3.6815156641032756E-3</v>
+        <v>3.7849290254544908E-3</v>
       </c>
       <c r="G4" s="25">
-        <v>2.8733624669311101E-3</v>
+        <v>9.3786078886417407E-3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="31">
-        <v>43415</v>
+        <v>43416</v>
       </c>
       <c r="B5" s="25">
-        <v>3.6194676472925462E-4</v>
+        <v>6.7218684878290127E-5</v>
       </c>
       <c r="C5" s="25">
-        <v>6.2048016810729349E-5</v>
+        <v>4.2658011557376432E-5</v>
       </c>
       <c r="D5" s="25">
-        <v>3.360934243914507E-3</v>
+        <v>1.8097338236462729E-3</v>
       </c>
       <c r="E5" s="25">
-        <v>3.8780010506705852E-3</v>
+        <v>1.9390005253352926E-3</v>
       </c>
       <c r="F5" s="25">
-        <v>3.7849290254544908E-3</v>
+        <v>1.9196105200819395E-3</v>
       </c>
       <c r="G5" s="25">
-        <v>9.3786078886417407E-3</v>
+        <v>6.5711741787783896E-3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="31">
-        <v>43416</v>
+        <v>43417</v>
       </c>
       <c r="B6" s="25">
-        <v>6.7218684878290127E-5</v>
+        <v>1.9390005253352921E-5</v>
       </c>
       <c r="C6" s="25">
-        <v>4.2658011557376432E-5</v>
+        <v>3.2316675422254876E-5</v>
       </c>
       <c r="D6" s="25">
-        <v>1.8097338236462729E-3</v>
+        <v>7.3682019962741107E-4</v>
       </c>
       <c r="E6" s="25">
-        <v>1.9390005253352926E-3</v>
+        <v>7.8852688030301885E-4</v>
       </c>
       <c r="F6" s="25">
-        <v>1.9196105200819395E-3</v>
+        <v>7.8852688030301885E-4</v>
       </c>
       <c r="G6" s="25">
-        <v>6.5711741787783896E-3</v>
+        <v>1.6733276286891401E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="31">
-        <v>43417</v>
+        <v>43418</v>
       </c>
       <c r="B7" s="25">
         <v>1.9390005253352921E-5</v>
       </c>
       <c r="C7" s="25">
-        <v>3.2316675422254876E-5</v>
+        <v>2.3268006304023508E-5</v>
       </c>
       <c r="D7" s="25">
-        <v>7.3682019962741107E-4</v>
+        <v>4.6536012608047012E-4</v>
       </c>
       <c r="E7" s="25">
-        <v>7.8852688030301885E-4</v>
+        <v>5.0414013658717596E-4</v>
       </c>
       <c r="F7" s="25">
-        <v>7.8852688030301885E-4</v>
+        <v>5.080181376378466E-4</v>
       </c>
       <c r="G7" s="25">
-        <v>1.6733276286891401E-2</v>
+        <v>2.5014189235818499E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="31">
-        <v>43418</v>
+        <v>43419</v>
       </c>
       <c r="B8" s="25">
-        <v>1.9390005253352921E-5</v>
+        <v>8.7901357148533266E-5</v>
       </c>
       <c r="C8" s="25">
-        <v>2.3268006304023508E-5</v>
+        <v>3.6194676472925452E-5</v>
       </c>
       <c r="D8" s="25">
-        <v>4.6536012608047012E-4</v>
+        <v>1.4219337185792142E-3</v>
       </c>
       <c r="E8" s="25">
-        <v>5.0414013658717596E-4</v>
+        <v>1.5512004202682336E-3</v>
       </c>
       <c r="F8" s="25">
-        <v>5.080181376378466E-4</v>
+        <v>1.5460297522006728E-3</v>
       </c>
       <c r="G8" s="25">
-        <v>2.5014189235818499E-2</v>
+        <v>1.37172891687236E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="31">
-        <v>43419</v>
+        <v>43420</v>
       </c>
       <c r="B9" s="25">
-        <v>8.7901357148533266E-5</v>
+        <v>9.0486691182313655E-5</v>
       </c>
       <c r="C9" s="25">
-        <v>3.6194676472925452E-5</v>
+        <v>6.5926017861399946E-5</v>
       </c>
       <c r="D9" s="25">
-        <v>1.4219337185792142E-3</v>
+        <v>2.5853340337803898E-3</v>
       </c>
       <c r="E9" s="25">
-        <v>1.5512004202682336E-3</v>
+        <v>2.7146007354694091E-3</v>
       </c>
       <c r="F9" s="25">
-        <v>1.5460297522006728E-3</v>
+        <v>2.7417467428241032E-3</v>
       </c>
       <c r="G9" s="25">
-        <v>1.37172891687236E-2</v>
+        <v>9.6193456182794099E-3</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="31">
-        <v>43420</v>
+        <v>43421</v>
       </c>
       <c r="B10" s="25">
-        <v>9.0486691182313655E-5</v>
+        <v>1.4219337185792145E-4</v>
       </c>
       <c r="C10" s="25">
-        <v>6.5926017861399946E-5</v>
+        <v>4.2658011557376432E-5</v>
       </c>
       <c r="D10" s="25">
-        <v>2.5853340337803898E-3</v>
+        <v>1.8097338236462729E-3</v>
       </c>
       <c r="E10" s="25">
-        <v>2.7146007354694091E-3</v>
+        <v>1.9390005253352926E-3</v>
       </c>
       <c r="F10" s="25">
-        <v>2.7417467428241032E-3</v>
+        <v>1.9945852070615707E-3</v>
       </c>
       <c r="G10" s="25">
-        <v>9.6193456182794099E-3</v>
+        <v>3.8951234076665203E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="31">
-        <v>43421</v>
+        <v>43422</v>
       </c>
       <c r="B11" s="25">
         <v>1.4219337185792145E-4</v>
       </c>
       <c r="C11" s="25">
-        <v>4.2658011557376432E-5</v>
+        <v>5.4292014709388175E-5</v>
       </c>
       <c r="D11" s="25">
-        <v>1.8097338236462729E-3</v>
+        <v>1.8355871639840766E-3</v>
       </c>
       <c r="E11" s="25">
         <v>1.9390005253352926E-3</v>
       </c>
       <c r="F11" s="25">
-        <v>1.9945852070615707E-3</v>
+        <v>2.0320725505513864E-3</v>
       </c>
       <c r="G11" s="25">
-        <v>3.8951234076665203E-2</v>
+        <v>2.61251783510086E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="31">
-        <v>43422</v>
+        <v>43423</v>
       </c>
       <c r="B12" s="25">
-        <v>1.4219337185792145E-4</v>
+        <v>1.034133613512156E-4</v>
       </c>
       <c r="C12" s="25">
-        <v>5.4292014709388175E-5</v>
+        <v>4.3950678574266633E-5</v>
       </c>
       <c r="D12" s="25">
-        <v>1.8355871639840766E-3</v>
+        <v>1.0858402941877636E-3</v>
       </c>
       <c r="E12" s="25">
-        <v>1.9390005253352926E-3</v>
+        <v>1.2280336660456853E-3</v>
       </c>
       <c r="F12" s="25">
-        <v>2.0320725505513864E-3</v>
+        <v>1.2332043341132459E-3</v>
       </c>
       <c r="G12" s="25">
-        <v>2.61251783510086E-2</v>
+        <v>3.7282780399230497E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="31">
-        <v>43423</v>
+        <v>43424</v>
       </c>
       <c r="B13" s="25">
-        <v>1.034133613512156E-4</v>
+        <v>2.8438674371584285E-5</v>
       </c>
       <c r="C13" s="25">
-        <v>4.3950678574266633E-5</v>
+        <v>9.5657359249874422E-6</v>
       </c>
       <c r="D13" s="25">
-        <v>1.0858402941877636E-3</v>
+        <v>2.9989874791852523E-4</v>
       </c>
       <c r="E13" s="25">
-        <v>1.2280336660456853E-3</v>
+        <v>3.3609342439145062E-4</v>
       </c>
       <c r="F13" s="25">
-        <v>1.2332043341132459E-3</v>
+        <v>3.3790315821509697E-4</v>
       </c>
       <c r="G13" s="25">
-        <v>3.7282780399230497E-2</v>
+        <v>0.228738722991462</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="31">
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="B14" s="25">
-        <v>2.8438674371584285E-5</v>
+        <v>1.4219337185792143E-5</v>
       </c>
       <c r="C14" s="25">
-        <v>9.5657359249874422E-6</v>
+        <v>5.1706680675607805E-6</v>
       </c>
       <c r="D14" s="25">
-        <v>2.9989874791852523E-4</v>
+        <v>1.5770537606060378E-4</v>
       </c>
       <c r="E14" s="25">
-        <v>3.3609342439145062E-4</v>
+        <v>1.6804671219572531E-4</v>
       </c>
       <c r="F14" s="25">
-        <v>3.3790315821509697E-4</v>
+        <v>1.770953813139567E-4</v>
       </c>
       <c r="G14" s="25">
-        <v>0.228738722991462</v>
+        <v>0.22990110773826999</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="31">
-        <v>43425</v>
+        <v>43426</v>
       </c>
       <c r="B15" s="25">
-        <v>1.4219337185792143E-5</v>
+        <v>1.5512004202682337E-5</v>
       </c>
       <c r="C15" s="25">
-        <v>5.1706680675607805E-6</v>
+        <v>6.7218684878290145E-6</v>
       </c>
       <c r="D15" s="25">
-        <v>1.5770537606060378E-4</v>
+        <v>3.878001050670584E-4</v>
       </c>
       <c r="E15" s="25">
-        <v>1.6804671219572531E-4</v>
+        <v>4.136534454048624E-4</v>
       </c>
       <c r="F15" s="25">
-        <v>1.770953813139567E-4</v>
+        <v>4.1003397775756976E-4</v>
       </c>
       <c r="G15" s="25">
-        <v>0.22990110773826999</v>
+        <v>8.3148015015551496E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="31">
-        <v>43426</v>
+        <v>43427</v>
       </c>
       <c r="B16" s="25">
-        <v>1.5512004202682337E-5</v>
+        <v>9.9535360300545016E-6</v>
       </c>
       <c r="C16" s="25">
-        <v>6.7218684878290145E-6</v>
+        <v>8.5316023114752873E-6</v>
       </c>
       <c r="D16" s="25">
-        <v>3.878001050670584E-4</v>
+        <v>3.3609342439145062E-4</v>
       </c>
       <c r="E16" s="25">
-        <v>4.136534454048624E-4</v>
+        <v>3.4902009456035267E-4</v>
       </c>
       <c r="F16" s="25">
-        <v>4.1003397775756976E-4</v>
+        <v>3.5457856273298042E-4</v>
       </c>
       <c r="G16" s="25">
-        <v>8.3148015015551496E-2</v>
+        <v>6.0942471554011397E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="31">
-        <v>43427</v>
+        <v>43428</v>
       </c>
       <c r="B17" s="25">
-        <v>9.9535360300545016E-6</v>
+        <v>1.5512004202682337E-5</v>
       </c>
       <c r="C17" s="25">
-        <v>8.5316023114752873E-6</v>
+        <v>1.6804671219572532E-5</v>
       </c>
       <c r="D17" s="25">
-        <v>3.3609342439145062E-4</v>
+        <v>4.136534454048624E-4</v>
       </c>
       <c r="E17" s="25">
-        <v>3.4902009456035267E-4</v>
+        <v>4.5243345591156823E-4</v>
       </c>
       <c r="F17" s="25">
-        <v>3.5457856273298042E-4</v>
+        <v>4.4597012082711726E-4</v>
       </c>
       <c r="G17" s="25">
-        <v>6.0942471554011397E-2</v>
+        <v>6.3413374318036494E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="31">
-        <v>43428</v>
+        <v>43429</v>
       </c>
       <c r="B18" s="25">
-        <v>1.5512004202682337E-5</v>
+        <v>1.6804671219572532E-5</v>
       </c>
       <c r="C18" s="25">
         <v>1.6804671219572532E-5</v>
       </c>
       <c r="D18" s="25">
-        <v>4.136534454048624E-4</v>
+        <v>6.2048016810729346E-4</v>
       </c>
       <c r="E18" s="25">
-        <v>4.5243345591156823E-4</v>
+        <v>6.4633350844509746E-4</v>
       </c>
       <c r="F18" s="25">
-        <v>4.4597012082711726E-4</v>
+        <v>6.5408951054643852E-4</v>
       </c>
       <c r="G18" s="25">
-        <v>6.3413374318036494E-2</v>
+        <v>5.86634942525334E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="31">
-        <v>43429</v>
+        <v>43430</v>
       </c>
       <c r="B19" s="25">
-        <v>1.6804671219572532E-5</v>
+        <v>1.5512004202682337E-5</v>
       </c>
       <c r="C19" s="25">
-        <v>1.6804671219572532E-5</v>
+        <v>2.8438674371584285E-5</v>
       </c>
       <c r="D19" s="25">
-        <v>6.2048016810729346E-4</v>
+        <v>8.5316023114752858E-4</v>
       </c>
       <c r="E19" s="25">
-        <v>6.4633350844509746E-4</v>
+        <v>8.9194024165423452E-4</v>
       </c>
       <c r="F19" s="25">
-        <v>6.5408951054643852E-4</v>
+        <v>8.9711090972179519E-4</v>
       </c>
       <c r="G19" s="25">
-        <v>5.86634942525334E-2</v>
+        <v>0.147500135140716</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="31">
-        <v>43430</v>
+        <v>43431</v>
       </c>
       <c r="B20" s="25">
-        <v>1.5512004202682337E-5</v>
+        <v>1.292667016890195E-5</v>
       </c>
       <c r="C20" s="25">
-        <v>2.8438674371584285E-5</v>
+        <v>1.6804671219572532E-5</v>
       </c>
       <c r="D20" s="25">
-        <v>8.5316023114752858E-4</v>
+        <v>9.4364692232984241E-4</v>
       </c>
       <c r="E20" s="25">
-        <v>8.9194024165423452E-4</v>
+        <v>9.695002626676463E-4</v>
       </c>
       <c r="F20" s="25">
-        <v>8.9711090972179519E-4</v>
+        <v>9.7337826371831694E-4</v>
       </c>
       <c r="G20" s="25">
-        <v>0.147500135140716</v>
+        <v>0.14183448146268099</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="31">
-        <v>43431</v>
+        <v>43432</v>
       </c>
       <c r="B21" s="25">
-        <v>1.292667016890195E-5</v>
+        <v>3.2316675422254875E-6</v>
       </c>
       <c r="C21" s="25">
-        <v>1.6804671219572532E-5</v>
+        <v>4.6536012608047022E-6</v>
       </c>
       <c r="D21" s="25">
-        <v>9.4364692232984241E-4</v>
+        <v>1.098766964356666E-4</v>
       </c>
       <c r="E21" s="25">
-        <v>9.695002626676463E-4</v>
+        <v>1.1763269853700773E-4</v>
       </c>
       <c r="F21" s="25">
-        <v>9.7337826371831694E-4</v>
+        <v>1.1776196523869679E-4</v>
       </c>
       <c r="G21" s="25">
-        <v>0.14183448146268099</v>
+        <v>0.14140377667337101</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="31">
-        <v>43432</v>
+        <v>43433</v>
       </c>
       <c r="B22" s="25">
-        <v>3.2316675422254875E-6</v>
+        <v>6.0755349793839165E-6</v>
       </c>
       <c r="C22" s="25">
-        <v>4.6536012608047022E-6</v>
+        <v>7.7560021013411686E-6</v>
       </c>
       <c r="D22" s="25">
-        <v>1.098766964356666E-4</v>
+        <v>4.2658011557376432E-5</v>
       </c>
       <c r="E22" s="25">
-        <v>1.1763269853700773E-4</v>
+        <v>5.6877348743168571E-5</v>
       </c>
       <c r="F22" s="25">
-        <v>1.1776196523869679E-4</v>
+        <v>5.6489548638101517E-5</v>
       </c>
       <c r="G22" s="25">
-        <v>0.14140377667337101</v>
+        <v>5.5464314338554199E-2</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="31">
-        <v>43433</v>
+        <v>43434</v>
       </c>
       <c r="B23" s="25">
-        <v>6.0755349793839165E-6</v>
+        <v>7.4974686979631307E-6</v>
       </c>
       <c r="C23" s="25">
-        <v>7.7560021013411686E-6</v>
+        <v>1.4219337185792143E-5</v>
       </c>
       <c r="D23" s="25">
-        <v>4.2658011557376432E-5</v>
+        <v>6.0755349793839161E-5</v>
       </c>
       <c r="E23" s="25">
-        <v>5.6877348743168571E-5</v>
+        <v>8.2730689080972488E-5</v>
       </c>
       <c r="F23" s="25">
-        <v>5.6489548638101517E-5</v>
+        <v>8.2472155677594438E-5</v>
       </c>
       <c r="G23" s="25">
-        <v>5.5464314338554199E-2</v>
+        <v>3.7783080558889202E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="31">
-        <v>43434</v>
+        <v>43435</v>
       </c>
       <c r="B24" s="25">
-        <v>7.4974686979631307E-6</v>
+        <v>1.5124204097615281E-5</v>
       </c>
       <c r="C24" s="25">
-        <v>1.4219337185792143E-5</v>
+        <v>1.9390005253352921E-5</v>
       </c>
       <c r="D24" s="25">
-        <v>6.0755349793839161E-5</v>
+        <v>1.4219337185792145E-4</v>
       </c>
       <c r="E24" s="25">
-        <v>8.2730689080972488E-5</v>
+        <v>1.8097338236462731E-4</v>
       </c>
       <c r="F24" s="25">
-        <v>8.2472155677594438E-5</v>
+        <v>1.7670758120888965E-4</v>
       </c>
       <c r="G24" s="25">
-        <v>3.7783080558889202E-2</v>
+        <v>6.73032781618155E-2</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="31">
-        <v>43435</v>
+        <v>43436</v>
       </c>
       <c r="B25" s="25">
-        <v>1.5124204097615281E-5</v>
+        <v>5.4292014709388175E-5</v>
       </c>
       <c r="C25" s="25">
-        <v>1.9390005253352921E-5</v>
+        <v>1.292667016890195E-5</v>
       </c>
       <c r="D25" s="25">
-        <v>1.4219337185792145E-4</v>
+        <v>2.3268006304023506E-4</v>
       </c>
       <c r="E25" s="25">
-        <v>1.8097338236462731E-4</v>
+        <v>2.9731341388474479E-4</v>
       </c>
       <c r="F25" s="25">
-        <v>1.7670758120888965E-4</v>
+        <v>2.9989874791852517E-4</v>
       </c>
       <c r="G25" s="25">
-        <v>6.73032781618155E-2</v>
+        <v>3.8245382498209399E-2</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="31">
-        <v>43436</v>
+        <v>43437</v>
       </c>
       <c r="B26" s="25">
-        <v>5.4292014709388175E-5</v>
+        <v>5.558468172627839E-5</v>
       </c>
       <c r="C26" s="25">
-        <v>1.292667016890195E-5</v>
+        <v>1.0858402941877637E-5</v>
       </c>
       <c r="D26" s="25">
-        <v>2.3268006304023506E-4</v>
+        <v>2.4560673320913706E-4</v>
       </c>
       <c r="E26" s="25">
-        <v>2.9731341388474479E-4</v>
+        <v>3.2316675422254873E-4</v>
       </c>
       <c r="F26" s="25">
-        <v>2.9989874791852517E-4</v>
+        <v>3.1204981787729308E-4</v>
       </c>
       <c r="G26" s="25">
-        <v>3.8245382498209399E-2</v>
+        <v>1.26867987117505E-2</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="31">
-        <v>43437</v>
+        <v>43438</v>
       </c>
       <c r="B27" s="25">
-        <v>5.558468172627839E-5</v>
+        <v>1.9390005253352921E-5</v>
       </c>
       <c r="C27" s="25">
-        <v>1.0858402941877637E-5</v>
+        <v>7.7560021013411686E-6</v>
       </c>
       <c r="D27" s="25">
-        <v>2.4560673320913706E-4</v>
+        <v>3.3609342439145063E-5</v>
       </c>
       <c r="E27" s="25">
-        <v>3.2316675422254873E-4</v>
+        <v>6.2048016810729349E-5</v>
       </c>
       <c r="F27" s="25">
-        <v>3.1204981787729308E-4</v>
+        <v>6.0755349793839154E-5</v>
       </c>
       <c r="G27" s="25">
-        <v>1.26867987117505E-2</v>
+        <v>1.40955332135656E-2</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="31">
-        <v>43438</v>
+        <v>43439</v>
       </c>
       <c r="B28" s="25">
-        <v>1.9390005253352921E-5</v>
+        <v>2.3268006304023508E-5</v>
       </c>
       <c r="C28" s="25">
-        <v>7.7560021013411686E-6</v>
+        <v>1.6804671219572532E-5</v>
       </c>
       <c r="D28" s="25">
-        <v>3.3609342439145063E-5</v>
+        <v>6.9804018912070516E-5</v>
       </c>
       <c r="E28" s="25">
-        <v>6.2048016810729349E-5</v>
+        <v>1.098766964356666E-4</v>
       </c>
       <c r="F28" s="25">
-        <v>6.0755349793839154E-5</v>
+        <v>1.0987669643566656E-4</v>
       </c>
       <c r="G28" s="25">
-        <v>1.40955332135656E-2</v>
+        <v>3.0127447413656298E-2</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="31">
-        <v>43439</v>
+        <v>43440</v>
       </c>
       <c r="B29" s="25">
-        <v>2.3268006304023508E-5</v>
+        <v>6.8511351895180335E-5</v>
       </c>
       <c r="C29" s="25">
-        <v>1.6804671219572532E-5</v>
+        <v>2.9731341388474483E-5</v>
       </c>
       <c r="D29" s="25">
-        <v>6.9804018912070516E-5</v>
+        <v>4.136534454048624E-4</v>
       </c>
       <c r="E29" s="25">
-        <v>1.098766964356666E-4</v>
+        <v>5.1706680675607801E-4</v>
       </c>
       <c r="F29" s="25">
-        <v>1.0987669643566656E-4</v>
+        <v>5.1189613868851723E-4</v>
       </c>
       <c r="G29" s="25">
-        <v>3.0127447413656298E-2</v>
+        <v>2.7292018286416898E-2</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="31">
-        <v>43440</v>
+        <v>43441</v>
       </c>
       <c r="B30" s="25">
-        <v>6.8511351895180335E-5</v>
+        <v>4.2658011557376432E-5</v>
       </c>
       <c r="C30" s="25">
-        <v>2.9731341388474483E-5</v>
+        <v>2.8438674371584285E-5</v>
       </c>
       <c r="D30" s="25">
-        <v>4.136534454048624E-4</v>
+        <v>2.4560673320913706E-4</v>
       </c>
       <c r="E30" s="25">
-        <v>5.1706680675607801E-4</v>
+        <v>3.1024008405364673E-4</v>
       </c>
       <c r="F30" s="25">
-        <v>5.1189613868851723E-4</v>
+        <v>3.1670341913809781E-4</v>
       </c>
       <c r="G30" s="25">
-        <v>2.7292018286416898E-2</v>
+        <v>5.2708593935022398E-2</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="31">
-        <v>43441</v>
+        <v>43442</v>
       </c>
       <c r="B31" s="25">
-        <v>4.2658011557376432E-5</v>
+        <v>1.0729136240188617E-4</v>
       </c>
       <c r="C31" s="25">
-        <v>2.8438674371584285E-5</v>
+        <v>5.17066806756078E-5</v>
       </c>
       <c r="D31" s="25">
-        <v>2.4560673320913706E-4</v>
+        <v>4.9121346641827412E-4</v>
       </c>
       <c r="E31" s="25">
-        <v>3.1024008405364673E-4</v>
+        <v>6.4633350844509746E-4</v>
       </c>
       <c r="F31" s="25">
-        <v>3.1670341913809781E-4</v>
+        <v>6.502115094957681E-4</v>
       </c>
       <c r="G31" s="25">
-        <v>5.2708593935022398E-2</v>
+        <v>0.139964512239381</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="31">
-        <v>43442</v>
+        <v>43443</v>
       </c>
       <c r="B32" s="25">
-        <v>1.0729136240188617E-4</v>
+        <v>2.7146007354694088E-5</v>
       </c>
       <c r="C32" s="25">
-        <v>5.17066806756078E-5</v>
+        <v>2.58533403378039E-5</v>
       </c>
       <c r="D32" s="25">
-        <v>4.9121346641827412E-4</v>
+        <v>7.7560021013411683E-5</v>
       </c>
       <c r="E32" s="25">
-        <v>6.4633350844509746E-4</v>
+        <v>1.292667016890195E-4</v>
       </c>
       <c r="F32" s="25">
-        <v>6.502115094957681E-4</v>
+        <v>1.3055936870590967E-4</v>
       </c>
       <c r="G32" s="25">
-        <v>0.139964512239381</v>
+        <v>0.125196900641111</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="31">
-        <v>43443</v>
+        <v>43444</v>
       </c>
       <c r="B33" s="25">
-        <v>2.7146007354694088E-5</v>
+        <v>3.1024008405364677E-6</v>
       </c>
       <c r="C33" s="25">
-        <v>2.58533403378039E-5</v>
+        <v>5.9462682776948967E-6</v>
       </c>
       <c r="D33" s="25">
-        <v>7.7560021013411683E-5</v>
+        <v>5.8170015760058769E-6</v>
       </c>
       <c r="E33" s="25">
-        <v>1.292667016890195E-4</v>
+        <v>1.5512004202682337E-5</v>
       </c>
       <c r="F33" s="25">
-        <v>1.3055936870590967E-4</v>
+        <v>1.4865670694237242E-5</v>
       </c>
       <c r="G33" s="25">
-        <v>0.125196900641111</v>
+        <v>6.6691800168083598E-2</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="31">
-        <v>43444</v>
+        <v>43445</v>
       </c>
       <c r="B34" s="25">
-        <v>3.1024008405364677E-6</v>
+        <v>6.8511351895180335E-6</v>
       </c>
       <c r="C34" s="25">
-        <v>5.9462682776948967E-6</v>
+        <v>9.8242693283654818E-6</v>
       </c>
       <c r="D34" s="25">
-        <v>5.8170015760058769E-6</v>
+        <v>1.9390005253352922E-6</v>
       </c>
       <c r="E34" s="25">
-        <v>1.5512004202682337E-5</v>
+        <v>3.6194676472925452E-5</v>
       </c>
       <c r="F34" s="25">
-        <v>1.4865670694237242E-5</v>
+        <v>1.8614405043218809E-5</v>
       </c>
       <c r="G34" s="25">
-        <v>6.6691800168083598E-2</v>
+        <v>0.145694033207942</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="31">
-        <v>43445</v>
+        <v>43446</v>
       </c>
       <c r="B35" s="25">
-        <v>6.8511351895180335E-6</v>
+        <v>8.143802206408228E-6</v>
       </c>
       <c r="C35" s="25">
-        <v>9.8242693283654818E-6</v>
+        <v>5.8170015760058769E-6</v>
       </c>
       <c r="D35" s="25">
-        <v>1.9390005253352922E-6</v>
+        <v>2.1975339287133316E-5</v>
       </c>
       <c r="E35" s="25">
         <v>3.6194676472925452E-5</v>
       </c>
       <c r="F35" s="25">
-        <v>1.8614405043218809E-5</v>
+        <v>3.5936143069547423E-5</v>
       </c>
       <c r="G35" s="25">
-        <v>0.145694033207942</v>
+        <v>0.11115874285383</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="31">
-        <v>43446</v>
+        <v>43447</v>
       </c>
       <c r="B36" s="25">
-        <v>8.143802206408228E-6</v>
+        <v>1.0082802731743521E-5</v>
       </c>
       <c r="C36" s="25">
-        <v>5.8170015760058769E-6</v>
+        <v>7.1096685928960714E-6</v>
       </c>
       <c r="D36" s="25">
-        <v>2.1975339287133316E-5</v>
+        <v>4.0072677523596043E-5</v>
       </c>
       <c r="E36" s="25">
-        <v>3.6194676472925452E-5</v>
+        <v>5.6877348743168571E-5</v>
       </c>
       <c r="F36" s="25">
-        <v>3.5936143069547423E-5</v>
+        <v>5.7265148848235632E-5</v>
       </c>
       <c r="G36" s="25">
-        <v>0.11115874285383</v>
+        <v>7.1360160147957902E-2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="31">
-        <v>43447</v>
+        <v>43448</v>
       </c>
       <c r="B37" s="25">
-        <v>1.0082802731743521E-5</v>
+        <v>1.0729136240188619E-5</v>
       </c>
       <c r="C37" s="25">
-        <v>7.1096685928960714E-6</v>
+        <v>1.2021803257078813E-5</v>
       </c>
       <c r="D37" s="25">
-        <v>4.0072677523596043E-5</v>
+        <v>3.6194676472925462E-4</v>
       </c>
       <c r="E37" s="25">
-        <v>5.6877348743168571E-5</v>
+        <v>3.878001050670584E-4</v>
       </c>
       <c r="F37" s="25">
-        <v>5.7265148848235632E-5</v>
+        <v>3.8469770422652207E-4</v>
       </c>
       <c r="G37" s="25">
-        <v>7.1360160147957902E-2</v>
+        <v>0.134450292872312</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="31">
-        <v>43448</v>
+        <v>43449</v>
       </c>
       <c r="B38" s="25">
-        <v>1.0729136240188619E-5</v>
+        <v>1.2668136765523909E-5</v>
       </c>
       <c r="C38" s="25">
-        <v>1.2021803257078813E-5</v>
+        <v>2.7146007354694088E-5</v>
       </c>
       <c r="D38" s="25">
-        <v>3.6194676472925462E-4</v>
+        <v>2.068267227024312E-4</v>
       </c>
       <c r="E38" s="25">
-        <v>3.878001050670584E-4</v>
+        <v>2.4560673320913706E-4</v>
       </c>
       <c r="F38" s="25">
-        <v>3.8469770422652207E-4</v>
+        <v>2.4664086682264921E-4</v>
       </c>
       <c r="G38" s="25">
-        <v>0.134450292872312</v>
+        <v>0.12731836646445799</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="31">
-        <v>43449</v>
+        <v>43450</v>
       </c>
       <c r="B39" s="25">
-        <v>1.2668136765523909E-5</v>
+        <v>7.4974686979631307E-6</v>
       </c>
       <c r="C39" s="25">
-        <v>2.7146007354694088E-5</v>
+        <v>1.4219337185792143E-5</v>
       </c>
       <c r="D39" s="25">
-        <v>2.068267227024312E-4</v>
+        <v>1.6804671219572532E-5</v>
       </c>
       <c r="E39" s="25">
-        <v>2.4560673320913706E-4</v>
+        <v>3.8780010506705841E-5</v>
       </c>
       <c r="F39" s="25">
-        <v>2.4664086682264921E-4</v>
+        <v>3.8521477103327805E-5</v>
       </c>
       <c r="G39" s="25">
-        <v>0.12731836646445799</v>
+        <v>0.12835376054341099</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="31">
-        <v>43450</v>
+        <v>43451</v>
       </c>
       <c r="B40" s="25">
-        <v>7.4974686979631307E-6</v>
+        <v>8.4023356097862659E-6</v>
       </c>
       <c r="C40" s="25">
-        <v>1.4219337185792143E-5</v>
+        <v>1.2668136765523909E-5</v>
       </c>
       <c r="D40" s="25">
-        <v>1.6804671219572532E-5</v>
+        <v>1.5512004202682337E-5</v>
       </c>
       <c r="E40" s="25">
-        <v>3.8780010506705841E-5</v>
+        <v>3.6194676472925452E-5</v>
       </c>
       <c r="F40" s="25">
-        <v>3.8521477103327805E-5</v>
+        <v>3.6582476577992507E-5</v>
       </c>
       <c r="G40" s="25">
-        <v>0.12835376054341099</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="31">
-        <v>43451</v>
-      </c>
-      <c r="B41" s="25">
-        <v>8.4023356097862659E-6</v>
-      </c>
-      <c r="C41" s="25">
-        <v>1.2668136765523909E-5</v>
-      </c>
-      <c r="D41" s="25">
-        <v>1.5512004202682337E-5</v>
-      </c>
-      <c r="E41" s="25">
-        <v>3.6194676472925452E-5</v>
-      </c>
-      <c r="F41" s="25">
-        <v>3.6582476577992507E-5</v>
-      </c>
-      <c r="G41" s="25">
         <v>8.5267981502381601E-2</v>
       </c>
     </row>
@@ -17339,969 +17297,946 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E68AD7-1011-4DE6-B10A-D94752D84ED3}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="44" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" style="44" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" style="44" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.81640625" style="44" customWidth="1"/>
-    <col min="6" max="6" width="11.26953125" style="48" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.08984375" style="48" customWidth="1"/>
-    <col min="8" max="8" width="13.08984375" style="44" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="44"/>
+    <col min="1" max="1" width="11.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.81640625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" style="25" customWidth="1"/>
+    <col min="8" max="8" width="13.08984375" style="9" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="25" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="47">
-        <v>43412</v>
-      </c>
-      <c r="B2" s="48">
+      <c r="A2" s="31">
+        <v>43413</v>
+      </c>
+      <c r="B2" s="25">
+        <v>3.6194676472925462E-4</v>
+      </c>
+      <c r="C2" s="25">
+        <v>2.58533403378039E-5</v>
+      </c>
+      <c r="D2" s="25">
+        <v>2.8438674371584283E-3</v>
+      </c>
+      <c r="E2" s="25">
+        <v>3.2316675422254877E-3</v>
+      </c>
+      <c r="F2" s="25">
+        <v>3.2316675422254869E-3</v>
+      </c>
+      <c r="G2" s="25">
+        <v>3.1858752699618301E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="31">
+        <v>43414</v>
+      </c>
+      <c r="B3" s="25">
+        <v>3.7487343489815651E-4</v>
+      </c>
+      <c r="C3" s="25">
+        <v>3.7487343489815654E-5</v>
+      </c>
+      <c r="D3" s="25">
+        <v>3.2316675422254877E-3</v>
+      </c>
+      <c r="E3" s="25">
+        <v>3.6194676472925459E-3</v>
+      </c>
+      <c r="F3" s="25">
+        <v>3.6440283206134599E-3</v>
+      </c>
+      <c r="G3" s="25">
+        <v>2.8733624669311101E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="31">
+        <v>43415</v>
+      </c>
+      <c r="B4" s="25">
+        <v>3.6194676472925462E-4</v>
+      </c>
+      <c r="C4" s="25">
+        <v>4.0072677523596043E-5</v>
+      </c>
+      <c r="D4" s="25">
+        <v>3.4902009456035258E-3</v>
+      </c>
+      <c r="E4" s="25">
+        <v>3.8780010506705852E-3</v>
+      </c>
+      <c r="F4" s="25">
+        <v>3.8922203878563764E-3</v>
+      </c>
+      <c r="G4" s="25">
+        <v>9.3786078886417407E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="31">
+        <v>43416</v>
+      </c>
+      <c r="B5" s="25">
+        <v>6.8511351895180335E-5</v>
+      </c>
+      <c r="C5" s="25">
+        <v>2.9731341388474483E-5</v>
+      </c>
+      <c r="D5" s="25">
+        <v>1.8097338236462729E-3</v>
+      </c>
+      <c r="E5" s="25">
+        <v>1.9390005253352926E-3</v>
+      </c>
+      <c r="F5" s="25">
+        <v>1.9079765169299277E-3</v>
+      </c>
+      <c r="G5" s="25">
+        <v>6.5711741787783896E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="31">
+        <v>43417</v>
+      </c>
+      <c r="B6" s="25">
+        <v>1.6804671219572532E-5</v>
+      </c>
+      <c r="C6" s="25">
+        <v>2.0682672270243122E-5</v>
+      </c>
+      <c r="D6" s="25">
+        <v>6.8511351895180319E-4</v>
+      </c>
+      <c r="E6" s="25">
+        <v>7.756002101341168E-4</v>
+      </c>
+      <c r="F6" s="25">
+        <v>7.2260086244161888E-4</v>
+      </c>
+      <c r="G6" s="25">
+        <v>1.6733276286891401E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="31">
+        <v>43418</v>
+      </c>
+      <c r="B7" s="25">
+        <v>1.5512004202682337E-5</v>
+      </c>
+      <c r="C7" s="25">
+        <v>5.2999347692498003E-6</v>
+      </c>
+      <c r="D7" s="25">
+        <v>4.7828679624937212E-4</v>
+      </c>
+      <c r="E7" s="25">
+        <v>4.9121346641827412E-4</v>
+      </c>
+      <c r="F7" s="25">
+        <v>4.9909873522130431E-4</v>
+      </c>
+      <c r="G7" s="25">
+        <v>2.5014189235818499E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="31">
+        <v>43419</v>
+      </c>
+      <c r="B8" s="25">
+        <v>8.4023356097862655E-5</v>
+      </c>
+      <c r="C8" s="25">
+        <v>1.8097338236462726E-5</v>
+      </c>
+      <c r="D8" s="25">
+        <v>1.4219337185792142E-3</v>
+      </c>
+      <c r="E8" s="25">
+        <v>1.5512004202682336E-3</v>
+      </c>
+      <c r="F8" s="25">
+        <v>1.5240544129135395E-3</v>
+      </c>
+      <c r="G8" s="25">
+        <v>1.37172891687236E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="31">
+        <v>43420</v>
+      </c>
+      <c r="B9" s="25">
+        <v>8.4023356097862655E-5</v>
+      </c>
+      <c r="C9" s="25">
+        <v>3.3609342439145063E-5</v>
+      </c>
+      <c r="D9" s="25">
+        <v>2.4560673320913706E-3</v>
+      </c>
+      <c r="E9" s="25">
+        <v>2.5853340337803898E-3</v>
+      </c>
+      <c r="F9" s="25">
+        <v>2.5737000306283783E-3</v>
+      </c>
+      <c r="G9" s="25">
+        <v>9.6193456182794099E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="31">
+        <v>43421</v>
+      </c>
+      <c r="B10" s="25">
+        <v>1.4219337185792145E-4</v>
+      </c>
+      <c r="C10" s="25">
+        <v>2.9731341388474483E-5</v>
+      </c>
+      <c r="D10" s="25">
+        <v>1.8097338236462729E-3</v>
+      </c>
+      <c r="E10" s="25">
+        <v>1.9390005253352926E-3</v>
+      </c>
+      <c r="F10" s="25">
+        <v>1.9816585368926691E-3</v>
+      </c>
+      <c r="G10" s="25">
+        <v>3.8951234076665203E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="31">
+        <v>43422</v>
+      </c>
+      <c r="B11" s="25">
+        <v>1.292667016890195E-4</v>
+      </c>
+      <c r="C11" s="25">
+        <v>2.7146007354694088E-5</v>
+      </c>
+      <c r="D11" s="25">
+        <v>1.8097338236462729E-3</v>
+      </c>
+      <c r="E11" s="25">
+        <v>1.9390005253352926E-3</v>
+      </c>
+      <c r="F11" s="25">
+        <v>1.9661465326899865E-3</v>
+      </c>
+      <c r="G11" s="25">
+        <v>2.61251783510086E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="31">
+        <v>43423</v>
+      </c>
+      <c r="B12" s="25">
+        <v>9.9535360300545016E-5</v>
+      </c>
+      <c r="C12" s="25">
+        <v>1.5512004202682337E-5</v>
+      </c>
+      <c r="D12" s="25">
+        <v>1.072913624018862E-3</v>
+      </c>
+      <c r="E12" s="25">
+        <v>1.1892536555389791E-3</v>
+      </c>
+      <c r="F12" s="25">
+        <v>1.1879609885220893E-3</v>
+      </c>
+      <c r="G12" s="25">
+        <v>3.7282780399230497E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="31">
+        <v>43424</v>
+      </c>
+      <c r="B13" s="25">
+        <v>2.7146007354694088E-5</v>
+      </c>
+      <c r="C13" s="25">
+        <v>3.4902009456035266E-6</v>
+      </c>
+      <c r="D13" s="25">
+        <v>2.9731341388474479E-4</v>
+      </c>
+      <c r="E13" s="25">
+        <v>3.3609342439145062E-4</v>
+      </c>
+      <c r="F13" s="25">
+        <v>3.2794962218504238E-4</v>
+      </c>
+      <c r="G13" s="25">
+        <v>0.228738722991462</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="31">
+        <v>43425</v>
+      </c>
+      <c r="B14" s="25">
+        <v>1.292667016890195E-5</v>
+      </c>
+      <c r="C14" s="25">
+        <v>2.1975339287133317E-6</v>
+      </c>
+      <c r="D14" s="25">
+        <v>1.5512004202682337E-4</v>
+      </c>
+      <c r="E14" s="25">
+        <v>1.6804671219572531E-4</v>
+      </c>
+      <c r="F14" s="25">
+        <v>1.7024424612443865E-4</v>
+      </c>
+      <c r="G14" s="25">
+        <v>0.22990110773826999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="31">
+        <v>43426</v>
+      </c>
+      <c r="B15" s="25">
+        <v>1.4219337185792143E-5</v>
+      </c>
+      <c r="C15" s="25">
+        <v>2.4560673320913705E-6</v>
+      </c>
+      <c r="D15" s="25">
+        <v>3.878001050670584E-4</v>
+      </c>
+      <c r="E15" s="25">
+        <v>4.007267752359604E-4</v>
+      </c>
+      <c r="F15" s="25">
+        <v>4.044755095849419E-4</v>
+      </c>
+      <c r="G15" s="25">
+        <v>8.3148015015551496E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="31">
+        <v>43427</v>
+      </c>
+      <c r="B16" s="25">
+        <v>9.1779358199203829E-6</v>
+      </c>
+      <c r="C16" s="25">
+        <v>2.1975339287133317E-6</v>
+      </c>
+      <c r="D16" s="25">
+        <v>3.3609342439145062E-4</v>
+      </c>
+      <c r="E16" s="25">
         <v>3.4902009456035267E-4</v>
       </c>
-      <c r="C2" s="48">
+      <c r="F16" s="25">
+        <v>3.4746889414008432E-4</v>
+      </c>
+      <c r="G16" s="25">
+        <v>6.0942471554011397E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="31">
+        <v>43428</v>
+      </c>
+      <c r="B17" s="25">
+        <v>1.292667016890195E-5</v>
+      </c>
+      <c r="C17" s="25">
+        <v>1.9390005253352922E-6</v>
+      </c>
+      <c r="D17" s="25">
+        <v>4.2658011557376429E-4</v>
+      </c>
+      <c r="E17" s="25">
+        <v>4.395067857426664E-4</v>
+      </c>
+      <c r="F17" s="25">
+        <v>4.4144578626800155E-4</v>
+      </c>
+      <c r="G17" s="25">
+        <v>6.3413374318036494E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="31">
+        <v>43429</v>
+      </c>
+      <c r="B18" s="25">
+        <v>1.4219337185792143E-5</v>
+      </c>
+      <c r="C18" s="25">
+        <v>3.1024008405364677E-6</v>
+      </c>
+      <c r="D18" s="25">
+        <v>6.2048016810729346E-4</v>
+      </c>
+      <c r="E18" s="25">
+        <v>6.3340683827619552E-4</v>
+      </c>
+      <c r="F18" s="25">
+        <v>6.3780190613362204E-4</v>
+      </c>
+      <c r="G18" s="25">
+        <v>5.86634942525334E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="31">
+        <v>43430</v>
+      </c>
+      <c r="B19" s="25">
+        <v>1.292667016890195E-5</v>
+      </c>
+      <c r="C19" s="25">
+        <v>1.6804671219572532E-5</v>
+      </c>
+      <c r="D19" s="25">
+        <v>8.273068908097248E-4</v>
+      </c>
+      <c r="E19" s="25">
+        <v>8.5316023114752858E-4</v>
+      </c>
+      <c r="F19" s="25">
+        <v>8.5703823219819932E-4</v>
+      </c>
+      <c r="G19" s="25">
+        <v>0.147500135140716</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="31">
+        <v>43431</v>
+      </c>
+      <c r="B20" s="25">
+        <v>1.2280336660456853E-5</v>
+      </c>
+      <c r="C20" s="25">
+        <v>1.2021803257078813E-5</v>
+      </c>
+      <c r="D20" s="25">
+        <v>9.4364692232984241E-4</v>
+      </c>
+      <c r="E20" s="25">
+        <v>9.695002626676463E-4</v>
+      </c>
+      <c r="F20" s="25">
+        <v>9.6794906224737811E-4</v>
+      </c>
+      <c r="G20" s="25">
+        <v>0.14183448146268099</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="31">
+        <v>43432</v>
+      </c>
+      <c r="B21" s="25">
+        <v>2.7146007354694092E-6</v>
+      </c>
+      <c r="C21" s="25">
+        <v>2.5853340337803902E-6</v>
+      </c>
+      <c r="D21" s="25">
+        <v>1.1116936345255678E-4</v>
+      </c>
+      <c r="E21" s="25">
+        <v>1.1634003152011753E-4</v>
+      </c>
+      <c r="F21" s="25">
+        <v>1.1646929822180658E-4</v>
+      </c>
+      <c r="G21" s="25">
+        <v>0.14140377667337101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="31">
+        <v>43433</v>
+      </c>
+      <c r="B22" s="25">
+        <v>5.1706680675607805E-6</v>
+      </c>
+      <c r="C22" s="25">
+        <v>3.3609342439145073E-6</v>
+      </c>
+      <c r="D22" s="25">
+        <v>4.3950678574266633E-5</v>
+      </c>
+      <c r="E22" s="25">
+        <v>5.2999347692497994E-5</v>
+      </c>
+      <c r="F22" s="25">
+        <v>5.2482280885741922E-5</v>
+      </c>
+      <c r="G22" s="25">
+        <v>5.5464314338554199E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="31">
+        <v>43434</v>
+      </c>
+      <c r="B23" s="25">
+        <v>5.5584681726278373E-6</v>
+      </c>
+      <c r="C23" s="25">
+        <v>4.7828679624937211E-6</v>
+      </c>
+      <c r="D23" s="25">
+        <v>5.9462682776948967E-5</v>
+      </c>
+      <c r="E23" s="25">
+        <v>6.9804018912070516E-5</v>
+      </c>
+      <c r="F23" s="25">
+        <v>6.9804018912070529E-5</v>
+      </c>
+      <c r="G23" s="25">
+        <v>3.7783080558889202E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="31">
+        <v>43435</v>
+      </c>
+      <c r="B24" s="25">
+        <v>1.9390005253352921E-5</v>
+      </c>
+      <c r="C24" s="25">
+        <v>4.1365344540486239E-6</v>
+      </c>
+      <c r="D24" s="25">
+        <v>1.4219337185792145E-4</v>
+      </c>
+      <c r="E24" s="25">
+        <v>1.6804671219572531E-4</v>
+      </c>
+      <c r="F24" s="25">
+        <v>1.65719911565323E-4</v>
+      </c>
+      <c r="G24" s="25">
+        <v>6.73032781618155E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="31">
+        <v>43436</v>
+      </c>
+      <c r="B25" s="25">
+        <v>5.0414013658717605E-5</v>
+      </c>
+      <c r="C25" s="25">
+        <v>8.5316023114752867E-7</v>
+      </c>
+      <c r="D25" s="25">
+        <v>2.3268006304023506E-4</v>
+      </c>
+      <c r="E25" s="25">
+        <v>2.843867437158429E-4</v>
+      </c>
+      <c r="F25" s="25">
+        <v>2.8394723693010021E-4</v>
+      </c>
+      <c r="G25" s="25">
+        <v>3.8245382498209399E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="31">
+        <v>43437</v>
+      </c>
+      <c r="B26" s="25">
+        <v>5.0414013658717605E-5</v>
+      </c>
+      <c r="C26" s="25">
+        <v>8.0145355047192084E-7</v>
+      </c>
+      <c r="D26" s="25">
+        <v>2.5853340337803901E-4</v>
+      </c>
+      <c r="E26" s="25">
+        <v>3.1024008405364673E-4</v>
+      </c>
+      <c r="F26" s="25">
+        <v>3.0974887058722854E-4</v>
+      </c>
+      <c r="G26" s="25">
+        <v>1.26867987117505E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="31">
+        <v>43438</v>
+      </c>
+      <c r="B27" s="25">
+        <v>1.6804671219572532E-5</v>
+      </c>
+      <c r="C27" s="25">
+        <v>1.292667016890195E-7</v>
+      </c>
+      <c r="D27" s="25">
+        <v>3.4902009456035258E-5</v>
+      </c>
+      <c r="E27" s="25">
+        <v>5.17066806756078E-5</v>
+      </c>
+      <c r="F27" s="25">
+        <v>5.1835947377296804E-5</v>
+      </c>
+      <c r="G27" s="25">
+        <v>1.40955332135656E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="31">
+        <v>43439</v>
+      </c>
+      <c r="B28" s="25">
+        <v>1.9390005253352921E-5</v>
+      </c>
+      <c r="C28" s="25">
+        <v>2.8438674371584291E-7</v>
+      </c>
+      <c r="D28" s="25">
+        <v>7.1096685928960724E-5</v>
+      </c>
+      <c r="E28" s="25">
+        <v>9.0486691182313655E-5</v>
+      </c>
+      <c r="F28" s="25">
+        <v>9.0771077926029496E-5</v>
+      </c>
+      <c r="G28" s="25">
+        <v>3.0127447413656298E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="31">
+        <v>43440</v>
+      </c>
+      <c r="B29" s="25">
+        <v>6.5926017861399946E-5</v>
+      </c>
+      <c r="C29" s="25">
+        <v>2.8438674371584291E-7</v>
+      </c>
+      <c r="D29" s="25">
+        <v>4.136534454048624E-4</v>
+      </c>
+      <c r="E29" s="25">
+        <v>4.7828679624937212E-4</v>
+      </c>
+      <c r="F29" s="25">
+        <v>4.7986385000997817E-4</v>
+      </c>
+      <c r="G29" s="25">
+        <v>2.7292018286416898E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="31">
+        <v>43441</v>
+      </c>
+      <c r="B30" s="25">
+        <v>3.7487343489815654E-5</v>
+      </c>
+      <c r="C30" s="25">
+        <v>1.2538870063834891E-6</v>
+      </c>
+      <c r="D30" s="25">
+        <v>2.4560673320913706E-4</v>
+      </c>
+      <c r="E30" s="25">
+        <v>2.843867437158429E-4</v>
+      </c>
+      <c r="F30" s="25">
+        <v>2.8434796370533619E-4</v>
+      </c>
+      <c r="G30" s="25">
+        <v>5.2708593935022398E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="31">
+        <v>43442</v>
+      </c>
+      <c r="B31" s="25">
+        <v>1.034133613512156E-4</v>
+      </c>
+      <c r="C31" s="25">
+        <v>2.8438674371584285E-5</v>
+      </c>
+      <c r="D31" s="25">
+        <v>4.9121346641827412E-4</v>
+      </c>
+      <c r="E31" s="25">
+        <v>6.2048016810729346E-4</v>
+      </c>
+      <c r="F31" s="25">
+        <v>6.2306550214107407E-4</v>
+      </c>
+      <c r="G31" s="25">
+        <v>0.139964512239381</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="31">
+        <v>43443</v>
+      </c>
+      <c r="B32" s="25">
+        <v>2.3268006304023508E-5</v>
+      </c>
+      <c r="C32" s="25">
+        <v>5.6877348743168562E-6</v>
+      </c>
+      <c r="D32" s="25">
+        <v>8.0145355047192085E-5</v>
+      </c>
+      <c r="E32" s="25">
+        <v>1.098766964356666E-4</v>
+      </c>
+      <c r="F32" s="25">
+        <v>1.0910109622553245E-4</v>
+      </c>
+      <c r="G32" s="25">
+        <v>0.125196900641111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="31">
+        <v>43444</v>
+      </c>
+      <c r="B33" s="25">
+        <v>1.9390005253352922E-6</v>
+      </c>
+      <c r="C33" s="25">
+        <v>3.748734348981565E-7</v>
+      </c>
+      <c r="D33" s="25">
+        <v>6.7218684878290145E-6</v>
+      </c>
+      <c r="E33" s="25">
+        <v>9.0486691182313631E-6</v>
+      </c>
+      <c r="F33" s="25">
+        <v>9.0357424480624623E-6</v>
+      </c>
+      <c r="G33" s="25">
+        <v>6.6691800168083598E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="31">
+        <v>43445</v>
+      </c>
+      <c r="B34" s="25">
+        <v>3.8780010506705843E-6</v>
+      </c>
+      <c r="C34" s="25">
+        <v>5.2999347692497994E-7</v>
+      </c>
+      <c r="D34" s="25">
         <v>2.1975339287133316E-5</v>
       </c>
-      <c r="D2" s="48">
-        <v>1.9390005253352926E-3</v>
-      </c>
-      <c r="E2" s="48">
-        <v>2.3268006304023509E-3</v>
-      </c>
-      <c r="F2" s="48">
-        <v>2.3099959591827788E-3</v>
-      </c>
-      <c r="G2" s="48" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="47">
-        <v>43413</v>
-      </c>
-      <c r="B3" s="48">
+      <c r="E34" s="25">
+        <v>2.7146007354694088E-5</v>
+      </c>
+      <c r="F34" s="25">
+        <v>2.6383333814728882E-5</v>
+      </c>
+      <c r="G34" s="25">
+        <v>0.145694033207942</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="31">
+        <v>43446</v>
+      </c>
+      <c r="B35" s="25">
+        <v>5.4292014709388184E-6</v>
+      </c>
+      <c r="C35" s="25">
+        <v>2.5853340337803899E-7</v>
+      </c>
+      <c r="D35" s="25">
+        <v>2.1975339287133316E-5</v>
+      </c>
+      <c r="E35" s="25">
+        <v>2.8438674371584285E-5</v>
+      </c>
+      <c r="F35" s="25">
+        <v>2.7663074161450174E-5</v>
+      </c>
+      <c r="G35" s="25">
+        <v>0.11115874285383</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="31">
+        <v>43447</v>
+      </c>
+      <c r="B36" s="25">
+        <v>8.4023356097862659E-6</v>
+      </c>
+      <c r="C36" s="25">
+        <v>2.326800630402351E-7</v>
+      </c>
+      <c r="D36" s="25">
+        <v>4.0072677523596043E-5</v>
+      </c>
+      <c r="E36" s="25">
+        <v>4.9121346641827411E-5</v>
+      </c>
+      <c r="F36" s="25">
+        <v>4.8707693196422545E-5</v>
+      </c>
+      <c r="G36" s="25">
+        <v>7.1360160147957902E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="31">
+        <v>43448</v>
+      </c>
+      <c r="B37" s="25">
+        <v>7.7560021013411686E-6</v>
+      </c>
+      <c r="C37" s="25">
+        <v>4.2658011557376434E-7</v>
+      </c>
+      <c r="D37" s="25">
         <v>3.6194676472925462E-4</v>
       </c>
-      <c r="C3" s="48">
-        <v>2.58533403378039E-5</v>
-      </c>
-      <c r="D3" s="48">
-        <v>2.8438674371584283E-3</v>
-      </c>
-      <c r="E3" s="48">
-        <v>3.2316675422254877E-3</v>
-      </c>
-      <c r="F3" s="48">
-        <v>3.2316675422254869E-3</v>
-      </c>
-      <c r="G3" s="48">
-        <v>3.1858752699618301E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="47">
-        <v>43414</v>
-      </c>
-      <c r="B4" s="48">
+      <c r="E37" s="25">
         <v>3.7487343489815651E-4</v>
       </c>
-      <c r="C4" s="48">
-        <v>3.7487343489815654E-5</v>
-      </c>
-      <c r="D4" s="48">
-        <v>3.2316675422254877E-3</v>
-      </c>
-      <c r="E4" s="48">
-        <v>3.6194676472925459E-3</v>
-      </c>
-      <c r="F4" s="48">
-        <v>3.6440283206134599E-3</v>
-      </c>
-      <c r="G4" s="48">
-        <v>2.8733624669311101E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="47">
-        <v>43415</v>
-      </c>
-      <c r="B5" s="48">
-        <v>3.6194676472925462E-4</v>
-      </c>
-      <c r="C5" s="48">
-        <v>4.0072677523596043E-5</v>
-      </c>
-      <c r="D5" s="48">
-        <v>3.4902009456035258E-3</v>
-      </c>
-      <c r="E5" s="48">
-        <v>3.8780010506705852E-3</v>
-      </c>
-      <c r="F5" s="48">
-        <v>3.8922203878563764E-3</v>
-      </c>
-      <c r="G5" s="48">
-        <v>9.3786078886417407E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="47">
-        <v>43416</v>
-      </c>
-      <c r="B6" s="48">
-        <v>6.8511351895180335E-5</v>
-      </c>
-      <c r="C6" s="48">
-        <v>2.9731341388474483E-5</v>
-      </c>
-      <c r="D6" s="48">
-        <v>1.8097338236462729E-3</v>
-      </c>
-      <c r="E6" s="48">
-        <v>1.9390005253352926E-3</v>
-      </c>
-      <c r="F6" s="48">
-        <v>1.9079765169299277E-3</v>
-      </c>
-      <c r="G6" s="48">
-        <v>6.5711741787783896E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="47">
-        <v>43417</v>
-      </c>
-      <c r="B7" s="48">
+      <c r="F37" s="25">
+        <v>3.7012934694616957E-4</v>
+      </c>
+      <c r="G37" s="25">
+        <v>0.134450292872312</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="31">
+        <v>43449</v>
+      </c>
+      <c r="B38" s="25">
+        <v>8.5316023114752873E-6</v>
+      </c>
+      <c r="C38" s="25">
+        <v>4.1365344540486232E-7</v>
+      </c>
+      <c r="D38" s="25">
+        <v>2.068267227024312E-4</v>
+      </c>
+      <c r="E38" s="25">
+        <v>2.197533928713332E-4</v>
+      </c>
+      <c r="F38" s="25">
+        <v>2.1577197845931134E-4</v>
+      </c>
+      <c r="G38" s="25">
+        <v>0.12731836646445799</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="31">
+        <v>43450</v>
+      </c>
+      <c r="B39" s="9">
+        <v>4.2658011557376437E-6</v>
+      </c>
+      <c r="C39" s="9">
+        <v>1.1246203046944695E-7</v>
+      </c>
+      <c r="D39" s="9">
         <v>1.6804671219572532E-5</v>
       </c>
-      <c r="C7" s="48">
+      <c r="E39" s="9">
         <v>2.0682672270243122E-5</v>
       </c>
-      <c r="D7" s="48">
-        <v>6.8511351895180319E-4</v>
-      </c>
-      <c r="E7" s="48">
-        <v>7.756002101341168E-4</v>
-      </c>
-      <c r="F7" s="48">
-        <v>7.2260086244161888E-4</v>
-      </c>
-      <c r="G7" s="48">
-        <v>1.6733276286891401E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="47">
-        <v>43418</v>
-      </c>
-      <c r="B8" s="48">
+      <c r="F39" s="25">
+        <v>2.118293440577962E-5</v>
+      </c>
+      <c r="G39" s="25">
+        <v>0.12835376054341099</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="31">
+        <v>43451</v>
+      </c>
+      <c r="B40" s="9">
+        <v>6.8511351895180335E-6</v>
+      </c>
+      <c r="C40" s="9">
+        <v>2.714600735469409E-7</v>
+      </c>
+      <c r="D40" s="9">
         <v>1.5512004202682337E-5</v>
       </c>
-      <c r="C8" s="48">
-        <v>5.2999347692498003E-6</v>
-      </c>
-      <c r="D8" s="48">
-        <v>4.7828679624937212E-4</v>
-      </c>
-      <c r="E8" s="48">
-        <v>4.9121346641827412E-4</v>
-      </c>
-      <c r="F8" s="48">
-        <v>4.9909873522130431E-4</v>
-      </c>
-      <c r="G8" s="48">
-        <v>2.5014189235818499E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="47">
-        <v>43419</v>
-      </c>
-      <c r="B9" s="48">
-        <v>8.4023356097862655E-5</v>
-      </c>
-      <c r="C9" s="48">
-        <v>1.8097338236462726E-5</v>
-      </c>
-      <c r="D9" s="48">
-        <v>1.4219337185792142E-3</v>
-      </c>
-      <c r="E9" s="48">
-        <v>1.5512004202682336E-3</v>
-      </c>
-      <c r="F9" s="48">
-        <v>1.5240544129135395E-3</v>
-      </c>
-      <c r="G9" s="48">
-        <v>1.37172891687236E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="47">
-        <v>43420</v>
-      </c>
-      <c r="B10" s="48">
-        <v>8.4023356097862655E-5</v>
-      </c>
-      <c r="C10" s="48">
-        <v>3.3609342439145063E-5</v>
-      </c>
-      <c r="D10" s="48">
-        <v>2.4560673320913706E-3</v>
-      </c>
-      <c r="E10" s="48">
-        <v>2.5853340337803898E-3</v>
-      </c>
-      <c r="F10" s="48">
-        <v>2.5737000306283783E-3</v>
-      </c>
-      <c r="G10" s="48">
-        <v>9.6193456182794099E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="47">
-        <v>43421</v>
-      </c>
-      <c r="B11" s="48">
-        <v>1.4219337185792145E-4</v>
-      </c>
-      <c r="C11" s="48">
-        <v>2.9731341388474483E-5</v>
-      </c>
-      <c r="D11" s="48">
-        <v>1.8097338236462729E-3</v>
-      </c>
-      <c r="E11" s="48">
-        <v>1.9390005253352926E-3</v>
-      </c>
-      <c r="F11" s="48">
-        <v>1.9816585368926691E-3</v>
-      </c>
-      <c r="G11" s="48">
-        <v>3.8951234076665203E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="47">
-        <v>43422</v>
-      </c>
-      <c r="B12" s="48">
-        <v>1.292667016890195E-4</v>
-      </c>
-      <c r="C12" s="48">
-        <v>2.7146007354694088E-5</v>
-      </c>
-      <c r="D12" s="48">
-        <v>1.8097338236462729E-3</v>
-      </c>
-      <c r="E12" s="48">
-        <v>1.9390005253352926E-3</v>
-      </c>
-      <c r="F12" s="48">
-        <v>1.9661465326899865E-3</v>
-      </c>
-      <c r="G12" s="48">
-        <v>2.61251783510086E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="47">
-        <v>43423</v>
-      </c>
-      <c r="B13" s="48">
-        <v>9.9535360300545016E-5</v>
-      </c>
-      <c r="C13" s="48">
-        <v>1.5512004202682337E-5</v>
-      </c>
-      <c r="D13" s="48">
-        <v>1.072913624018862E-3</v>
-      </c>
-      <c r="E13" s="48">
-        <v>1.1892536555389791E-3</v>
-      </c>
-      <c r="F13" s="48">
-        <v>1.1879609885220893E-3</v>
-      </c>
-      <c r="G13" s="48">
-        <v>3.7282780399230497E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="47">
-        <v>43424</v>
-      </c>
-      <c r="B14" s="48">
-        <v>2.7146007354694088E-5</v>
-      </c>
-      <c r="C14" s="48">
-        <v>3.4902009456035266E-6</v>
-      </c>
-      <c r="D14" s="48">
-        <v>2.9731341388474479E-4</v>
-      </c>
-      <c r="E14" s="48">
-        <v>3.3609342439145062E-4</v>
-      </c>
-      <c r="F14" s="48">
-        <v>3.2794962218504238E-4</v>
-      </c>
-      <c r="G14" s="48">
-        <v>0.228738722991462</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="47">
-        <v>43425</v>
-      </c>
-      <c r="B15" s="48">
-        <v>1.292667016890195E-5</v>
-      </c>
-      <c r="C15" s="48">
-        <v>2.1975339287133317E-6</v>
-      </c>
-      <c r="D15" s="48">
-        <v>1.5512004202682337E-4</v>
-      </c>
-      <c r="E15" s="48">
-        <v>1.6804671219572531E-4</v>
-      </c>
-      <c r="F15" s="48">
-        <v>1.7024424612443865E-4</v>
-      </c>
-      <c r="G15" s="48">
-        <v>0.22990110773826999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="47">
-        <v>43426</v>
-      </c>
-      <c r="B16" s="48">
-        <v>1.4219337185792143E-5</v>
-      </c>
-      <c r="C16" s="48">
-        <v>2.4560673320913705E-6</v>
-      </c>
-      <c r="D16" s="48">
-        <v>3.878001050670584E-4</v>
-      </c>
-      <c r="E16" s="48">
-        <v>4.007267752359604E-4</v>
-      </c>
-      <c r="F16" s="48">
-        <v>4.044755095849419E-4</v>
-      </c>
-      <c r="G16" s="48">
-        <v>8.3148015015551496E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="47">
-        <v>43427</v>
-      </c>
-      <c r="B17" s="48">
-        <v>9.1779358199203829E-6</v>
-      </c>
-      <c r="C17" s="48">
-        <v>2.1975339287133317E-6</v>
-      </c>
-      <c r="D17" s="48">
-        <v>3.3609342439145062E-4</v>
-      </c>
-      <c r="E17" s="48">
-        <v>3.4902009456035267E-4</v>
-      </c>
-      <c r="F17" s="48">
-        <v>3.4746889414008432E-4</v>
-      </c>
-      <c r="G17" s="48">
-        <v>6.0942471554011397E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="47">
-        <v>43428</v>
-      </c>
-      <c r="B18" s="48">
-        <v>1.292667016890195E-5</v>
-      </c>
-      <c r="C18" s="48">
-        <v>1.9390005253352922E-6</v>
-      </c>
-      <c r="D18" s="48">
-        <v>4.2658011557376429E-4</v>
-      </c>
-      <c r="E18" s="48">
-        <v>4.395067857426664E-4</v>
-      </c>
-      <c r="F18" s="48">
-        <v>4.4144578626800155E-4</v>
-      </c>
-      <c r="G18" s="48">
-        <v>6.3413374318036494E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="47">
-        <v>43429</v>
-      </c>
-      <c r="B19" s="48">
-        <v>1.4219337185792143E-5</v>
-      </c>
-      <c r="C19" s="48">
-        <v>3.1024008405364677E-6</v>
-      </c>
-      <c r="D19" s="48">
-        <v>6.2048016810729346E-4</v>
-      </c>
-      <c r="E19" s="48">
-        <v>6.3340683827619552E-4</v>
-      </c>
-      <c r="F19" s="48">
-        <v>6.3780190613362204E-4</v>
-      </c>
-      <c r="G19" s="48">
-        <v>5.86634942525334E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="47">
-        <v>43430</v>
-      </c>
-      <c r="B20" s="48">
-        <v>1.292667016890195E-5</v>
-      </c>
-      <c r="C20" s="48">
-        <v>1.6804671219572532E-5</v>
-      </c>
-      <c r="D20" s="48">
-        <v>8.273068908097248E-4</v>
-      </c>
-      <c r="E20" s="48">
-        <v>8.5316023114752858E-4</v>
-      </c>
-      <c r="F20" s="48">
-        <v>8.5703823219819932E-4</v>
-      </c>
-      <c r="G20" s="48">
-        <v>0.147500135140716</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="47">
-        <v>43431</v>
-      </c>
-      <c r="B21" s="48">
-        <v>1.2280336660456853E-5</v>
-      </c>
-      <c r="C21" s="48">
-        <v>1.2021803257078813E-5</v>
-      </c>
-      <c r="D21" s="48">
-        <v>9.4364692232984241E-4</v>
-      </c>
-      <c r="E21" s="48">
-        <v>9.695002626676463E-4</v>
-      </c>
-      <c r="F21" s="48">
-        <v>9.6794906224737811E-4</v>
-      </c>
-      <c r="G21" s="48">
-        <v>0.14183448146268099</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="47">
-        <v>43432</v>
-      </c>
-      <c r="B22" s="48">
-        <v>2.7146007354694092E-6</v>
-      </c>
-      <c r="C22" s="48">
-        <v>2.5853340337803902E-6</v>
-      </c>
-      <c r="D22" s="48">
-        <v>1.1116936345255678E-4</v>
-      </c>
-      <c r="E22" s="48">
-        <v>1.1634003152011753E-4</v>
-      </c>
-      <c r="F22" s="48">
-        <v>1.1646929822180658E-4</v>
-      </c>
-      <c r="G22" s="48">
-        <v>0.14140377667337101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="47">
-        <v>43433</v>
-      </c>
-      <c r="B23" s="48">
-        <v>5.1706680675607805E-6</v>
-      </c>
-      <c r="C23" s="48">
-        <v>3.3609342439145073E-6</v>
-      </c>
-      <c r="D23" s="48">
-        <v>4.3950678574266633E-5</v>
-      </c>
-      <c r="E23" s="48">
-        <v>5.2999347692497994E-5</v>
-      </c>
-      <c r="F23" s="48">
-        <v>5.2482280885741922E-5</v>
-      </c>
-      <c r="G23" s="48">
-        <v>5.5464314338554199E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="47">
-        <v>43434</v>
-      </c>
-      <c r="B24" s="48">
-        <v>5.5584681726278373E-6</v>
-      </c>
-      <c r="C24" s="48">
-        <v>4.7828679624937211E-6</v>
-      </c>
-      <c r="D24" s="48">
-        <v>5.9462682776948967E-5</v>
-      </c>
-      <c r="E24" s="48">
-        <v>6.9804018912070516E-5</v>
-      </c>
-      <c r="F24" s="48">
-        <v>6.9804018912070529E-5</v>
-      </c>
-      <c r="G24" s="48">
-        <v>3.7783080558889202E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="47">
-        <v>43435</v>
-      </c>
-      <c r="B25" s="48">
-        <v>1.9390005253352921E-5</v>
-      </c>
-      <c r="C25" s="48">
-        <v>4.1365344540486239E-6</v>
-      </c>
-      <c r="D25" s="48">
-        <v>1.4219337185792145E-4</v>
-      </c>
-      <c r="E25" s="48">
-        <v>1.6804671219572531E-4</v>
-      </c>
-      <c r="F25" s="48">
-        <v>1.65719911565323E-4</v>
-      </c>
-      <c r="G25" s="48">
-        <v>6.73032781618155E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="47">
-        <v>43436</v>
-      </c>
-      <c r="B26" s="48">
-        <v>5.0414013658717605E-5</v>
-      </c>
-      <c r="C26" s="48">
-        <v>8.5316023114752867E-7</v>
-      </c>
-      <c r="D26" s="48">
-        <v>2.3268006304023506E-4</v>
-      </c>
-      <c r="E26" s="48">
-        <v>2.843867437158429E-4</v>
-      </c>
-      <c r="F26" s="48">
-        <v>2.8394723693010021E-4</v>
-      </c>
-      <c r="G26" s="48">
-        <v>3.8245382498209399E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="47">
-        <v>43437</v>
-      </c>
-      <c r="B27" s="48">
-        <v>5.0414013658717605E-5</v>
-      </c>
-      <c r="C27" s="48">
-        <v>8.0145355047192084E-7</v>
-      </c>
-      <c r="D27" s="48">
-        <v>2.5853340337803901E-4</v>
-      </c>
-      <c r="E27" s="48">
-        <v>3.1024008405364673E-4</v>
-      </c>
-      <c r="F27" s="48">
-        <v>3.0974887058722854E-4</v>
-      </c>
-      <c r="G27" s="48">
-        <v>1.26867987117505E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="47">
-        <v>43438</v>
-      </c>
-      <c r="B28" s="48">
-        <v>1.6804671219572532E-5</v>
-      </c>
-      <c r="C28" s="48">
-        <v>1.292667016890195E-7</v>
-      </c>
-      <c r="D28" s="48">
-        <v>3.4902009456035258E-5</v>
-      </c>
-      <c r="E28" s="48">
-        <v>5.17066806756078E-5</v>
-      </c>
-      <c r="F28" s="48">
-        <v>5.1835947377296804E-5</v>
-      </c>
-      <c r="G28" s="48">
-        <v>1.40955332135656E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="47">
-        <v>43439</v>
-      </c>
-      <c r="B29" s="48">
-        <v>1.9390005253352921E-5</v>
-      </c>
-      <c r="C29" s="48">
-        <v>2.8438674371584291E-7</v>
-      </c>
-      <c r="D29" s="48">
-        <v>7.1096685928960724E-5</v>
-      </c>
-      <c r="E29" s="48">
-        <v>9.0486691182313655E-5</v>
-      </c>
-      <c r="F29" s="48">
-        <v>9.0771077926029496E-5</v>
-      </c>
-      <c r="G29" s="48">
-        <v>3.0127447413656298E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="47">
-        <v>43440</v>
-      </c>
-      <c r="B30" s="48">
-        <v>6.5926017861399946E-5</v>
-      </c>
-      <c r="C30" s="48">
-        <v>2.8438674371584291E-7</v>
-      </c>
-      <c r="D30" s="48">
-        <v>4.136534454048624E-4</v>
-      </c>
-      <c r="E30" s="48">
-        <v>4.7828679624937212E-4</v>
-      </c>
-      <c r="F30" s="48">
-        <v>4.7986385000997817E-4</v>
-      </c>
-      <c r="G30" s="48">
-        <v>2.7292018286416898E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="47">
-        <v>43441</v>
-      </c>
-      <c r="B31" s="48">
-        <v>3.7487343489815654E-5</v>
-      </c>
-      <c r="C31" s="48">
-        <v>1.2538870063834891E-6</v>
-      </c>
-      <c r="D31" s="48">
-        <v>2.4560673320913706E-4</v>
-      </c>
-      <c r="E31" s="48">
-        <v>2.843867437158429E-4</v>
-      </c>
-      <c r="F31" s="48">
-        <v>2.8434796370533619E-4</v>
-      </c>
-      <c r="G31" s="48">
-        <v>5.2708593935022398E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="47">
-        <v>43442</v>
-      </c>
-      <c r="B32" s="48">
-        <v>1.034133613512156E-4</v>
-      </c>
-      <c r="C32" s="48">
-        <v>2.8438674371584285E-5</v>
-      </c>
-      <c r="D32" s="48">
-        <v>4.9121346641827412E-4</v>
-      </c>
-      <c r="E32" s="48">
-        <v>6.2048016810729346E-4</v>
-      </c>
-      <c r="F32" s="48">
-        <v>6.2306550214107407E-4</v>
-      </c>
-      <c r="G32" s="48">
-        <v>0.139964512239381</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="47">
-        <v>43443</v>
-      </c>
-      <c r="B33" s="48">
-        <v>2.3268006304023508E-5</v>
-      </c>
-      <c r="C33" s="48">
-        <v>5.6877348743168562E-6</v>
-      </c>
-      <c r="D33" s="48">
-        <v>8.0145355047192085E-5</v>
-      </c>
-      <c r="E33" s="48">
-        <v>1.098766964356666E-4</v>
-      </c>
-      <c r="F33" s="48">
-        <v>1.0910109622553245E-4</v>
-      </c>
-      <c r="G33" s="48">
-        <v>0.125196900641111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="47">
-        <v>43444</v>
-      </c>
-      <c r="B34" s="48">
-        <v>1.9390005253352922E-6</v>
-      </c>
-      <c r="C34" s="48">
-        <v>3.748734348981565E-7</v>
-      </c>
-      <c r="D34" s="48">
-        <v>6.7218684878290145E-6</v>
-      </c>
-      <c r="E34" s="48">
-        <v>9.0486691182313631E-6</v>
-      </c>
-      <c r="F34" s="48">
-        <v>9.0357424480624623E-6</v>
-      </c>
-      <c r="G34" s="48">
-        <v>6.6691800168083598E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="47">
-        <v>43445</v>
-      </c>
-      <c r="B35" s="48">
-        <v>3.8780010506705843E-6</v>
-      </c>
-      <c r="C35" s="48">
-        <v>5.2999347692497994E-7</v>
-      </c>
-      <c r="D35" s="48">
+      <c r="E40" s="9">
         <v>2.1975339287133316E-5</v>
       </c>
-      <c r="E35" s="48">
-        <v>2.7146007354694088E-5</v>
-      </c>
-      <c r="F35" s="48">
-        <v>2.6383333814728882E-5</v>
-      </c>
-      <c r="G35" s="48">
-        <v>0.145694033207942</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="47">
-        <v>43446</v>
-      </c>
-      <c r="B36" s="48">
-        <v>5.4292014709388184E-6</v>
-      </c>
-      <c r="C36" s="48">
-        <v>2.5853340337803899E-7</v>
-      </c>
-      <c r="D36" s="48">
-        <v>2.1975339287133316E-5</v>
-      </c>
-      <c r="E36" s="48">
-        <v>2.8438674371584285E-5</v>
-      </c>
-      <c r="F36" s="48">
-        <v>2.7663074161450174E-5</v>
-      </c>
-      <c r="G36" s="48">
-        <v>0.11115874285383</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="47">
-        <v>43447</v>
-      </c>
-      <c r="B37" s="48">
-        <v>8.4023356097862659E-6</v>
-      </c>
-      <c r="C37" s="48">
-        <v>2.326800630402351E-7</v>
-      </c>
-      <c r="D37" s="48">
-        <v>4.0072677523596043E-5</v>
-      </c>
-      <c r="E37" s="48">
-        <v>4.9121346641827411E-5</v>
-      </c>
-      <c r="F37" s="48">
-        <v>4.8707693196422545E-5</v>
-      </c>
-      <c r="G37" s="48">
-        <v>7.1360160147957902E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="47">
-        <v>43448</v>
-      </c>
-      <c r="B38" s="48">
-        <v>7.7560021013411686E-6</v>
-      </c>
-      <c r="C38" s="48">
-        <v>4.2658011557376434E-7</v>
-      </c>
-      <c r="D38" s="48">
-        <v>3.6194676472925462E-4</v>
-      </c>
-      <c r="E38" s="48">
-        <v>3.7487343489815651E-4</v>
-      </c>
-      <c r="F38" s="48">
-        <v>3.7012934694616957E-4</v>
-      </c>
-      <c r="G38" s="48">
-        <v>0.134450292872312</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="47">
-        <v>43449</v>
-      </c>
-      <c r="B39" s="48">
-        <v>8.5316023114752873E-6</v>
-      </c>
-      <c r="C39" s="48">
-        <v>4.1365344540486232E-7</v>
-      </c>
-      <c r="D39" s="48">
-        <v>2.068267227024312E-4</v>
-      </c>
-      <c r="E39" s="48">
-        <v>2.197533928713332E-4</v>
-      </c>
-      <c r="F39" s="48">
-        <v>2.1577197845931134E-4</v>
-      </c>
-      <c r="G39" s="48">
-        <v>0.12731836646445799</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="47">
-        <v>43450</v>
-      </c>
-      <c r="B40" s="44">
-        <v>4.2658011557376437E-6</v>
-      </c>
-      <c r="C40" s="44">
-        <v>1.1246203046944695E-7</v>
-      </c>
-      <c r="D40" s="44">
-        <v>1.6804671219572532E-5</v>
-      </c>
-      <c r="E40" s="44">
-        <v>2.0682672270243122E-5</v>
-      </c>
-      <c r="F40" s="48">
-        <v>2.118293440577962E-5</v>
-      </c>
-      <c r="G40" s="48">
-        <v>0.12835376054341099</v>
+      <c r="F40" s="25">
+        <v>2.2634599465747313E-5</v>
+      </c>
+      <c r="G40" s="25">
+        <v>8.5267981502381601E-2</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="47">
-        <v>43451</v>
-      </c>
-      <c r="B41" s="44">
-        <v>6.8511351895180335E-6</v>
-      </c>
-      <c r="C41" s="44">
-        <v>2.714600735469409E-7</v>
-      </c>
-      <c r="D41" s="44">
-        <v>1.5512004202682337E-5</v>
-      </c>
-      <c r="E41" s="44">
-        <v>2.1975339287133316E-5</v>
-      </c>
-      <c r="F41" s="48">
-        <v>2.2634599465747313E-5</v>
-      </c>
-      <c r="G41" s="48">
-        <v>8.5267981502381601E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F42" s="44"/>
+      <c r="F41" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>